<commit_message>
Add admin link to navigation and update contact form layout for improved usability
</commit_message>
<xml_diff>
--- a/ManualGuide.xlsx
+++ b/ManualGuide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kghte\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kghte\Desktop\2Lakhs\my_django_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Manual" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Procedure</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t xml:space="preserve"> when you reset migrate, you have to go the 2nd sheet and re-create admin acc again firstly.</t>
+  </si>
+  <si>
+    <t>pip install django-jazzmin</t>
   </si>
 </sst>
 </file>
@@ -347,20 +350,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,13 +1067,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>180</xdr:row>
       <xdr:rowOff>88901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>181</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>109898</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1079,7 +1083,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2203450" y="30670501"/>
+          <a:off x="2203450" y="33248601"/>
           <a:ext cx="6400800" cy="2783247"/>
           <a:chOff x="2203450" y="30670501"/>
           <a:chExt cx="6400800" cy="2783247"/>
@@ -1229,13 +1233,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>98425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>178</xdr:row>
+      <xdr:row>192</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1272,6 +1276,44 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>148546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="30835600"/>
+          <a:ext cx="5943600" cy="1551896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1394,19 +1436,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>101600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>127001</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>127202</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>121663</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1419,8 +1461,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="685800" y="1047751"/>
-          <a:ext cx="6400800" cy="2762451"/>
+          <a:off x="711200" y="1054100"/>
+          <a:ext cx="5943600" cy="2566413"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1817,9 +1859,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S179"/>
+  <dimension ref="A1:S193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A181" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1838,15 +1880,15 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
@@ -1889,91 +1931,91 @@
       <c r="B80">
         <v>6</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C81" s="2"/>
-      <c r="D81" s="3" t="s">
+      <c r="D81" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E81" s="3"/>
+      <c r="E81" s="6"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84">
         <v>7</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7"/>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B101">
         <v>8</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E102" s="3"/>
+      <c r="E102" s="6"/>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B120">
         <v>9</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E121" s="3"/>
+      <c r="E121" s="6"/>
     </row>
     <row r="144" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B144">
         <v>10</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D144" s="4"/>
-      <c r="E144" s="4"/>
-      <c r="F144" s="4"/>
-      <c r="G144" s="4"/>
-      <c r="H144" s="4"/>
-      <c r="I144" s="4"/>
-      <c r="J144" s="4"/>
-      <c r="K144" s="4"/>
-      <c r="L144" s="4"/>
-      <c r="M144" s="4"/>
-      <c r="N144" s="4"/>
-      <c r="O144" s="4"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
+      <c r="F144" s="8"/>
+      <c r="G144" s="8"/>
+      <c r="H144" s="8"/>
+      <c r="I144" s="8"/>
+      <c r="J144" s="8"/>
+      <c r="K144" s="8"/>
+      <c r="L144" s="8"/>
+      <c r="M144" s="8"/>
+      <c r="N144" s="8"/>
+      <c r="O144" s="8"/>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B146">
@@ -1984,117 +2026,180 @@
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D147" s="3" t="s">
+      <c r="D147" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E147" s="3"/>
+      <c r="E147" s="6"/>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D148" s="5"/>
-      <c r="E148" s="5"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D149" s="5"/>
-      <c r="E149" s="5"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D150" s="5"/>
-      <c r="E150" s="5"/>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D151" s="5"/>
-      <c r="E151" s="5"/>
+      <c r="D151" s="3"/>
+      <c r="E151" s="3"/>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D152" s="5"/>
-      <c r="E152" s="5"/>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D153" s="5"/>
-      <c r="E153" s="5"/>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D154" s="5"/>
-      <c r="E154" s="5"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D155" s="5"/>
-      <c r="E155" s="5"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D156" s="5"/>
-      <c r="E156" s="5"/>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D157" s="5"/>
-      <c r="E157" s="5"/>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D158" s="5"/>
-      <c r="E158" s="5"/>
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D159" s="5"/>
-      <c r="E159" s="5"/>
+      <c r="D159" s="3"/>
+      <c r="E159" s="3"/>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D160" s="5"/>
-      <c r="E160" s="5"/>
-    </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D161" s="5"/>
-      <c r="E161" s="5"/>
-    </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D162" s="5"/>
-      <c r="E162" s="5"/>
-    </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D163" s="5"/>
-      <c r="E163" s="5"/>
-    </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D164" s="5"/>
-      <c r="E164" s="5"/>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B165">
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D161" s="3"/>
+      <c r="E161" s="3"/>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D162" s="3"/>
+      <c r="E162" s="3"/>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D163" s="3"/>
+      <c r="E163" s="3"/>
+    </row>
+    <row r="164" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+    </row>
+    <row r="165" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B165" s="1">
         <v>12</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D166" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E166" s="6"/>
+    </row>
+    <row r="167" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D167" s="3"/>
+      <c r="E167" s="3"/>
+    </row>
+    <row r="168" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D168" s="3"/>
+      <c r="E168" s="3"/>
+    </row>
+    <row r="169" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D169" s="3"/>
+      <c r="E169" s="3"/>
+    </row>
+    <row r="170" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+    </row>
+    <row r="171" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D171" s="3"/>
+      <c r="E171" s="3"/>
+    </row>
+    <row r="172" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D172" s="3"/>
+      <c r="E172" s="3"/>
+    </row>
+    <row r="173" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D173" s="3"/>
+      <c r="E173" s="3"/>
+    </row>
+    <row r="174" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D174" s="3"/>
+      <c r="E174" s="3"/>
+    </row>
+    <row r="175" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D175" s="3"/>
+      <c r="E175" s="3"/>
+    </row>
+    <row r="176" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D176" s="3"/>
+      <c r="E176" s="3"/>
+    </row>
+    <row r="177" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D177" s="3"/>
+      <c r="E177" s="3"/>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="D178" s="3"/>
+      <c r="E178" s="3"/>
+    </row>
+    <row r="179" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B179">
+        <v>13</v>
+      </c>
+      <c r="C179" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D166" s="3" t="s">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="D180" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E166" s="3"/>
-      <c r="F166" s="3"/>
-    </row>
-    <row r="179" spans="15:19" x14ac:dyDescent="0.35">
-      <c r="O179" s="1" t="s">
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
+    </row>
+    <row r="193" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O193" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P179" s="1"/>
-      <c r="Q179" s="1"/>
-      <c r="R179" s="1"/>
-      <c r="S179" s="1"/>
+      <c r="P193" s="7"/>
+      <c r="Q193" s="7"/>
+      <c r="R193" s="7"/>
+      <c r="S193" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D166:F166"/>
+  <mergeCells count="13">
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C80:H80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="C84:I84"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D180:F180"/>
     <mergeCell ref="D147:E147"/>
-    <mergeCell ref="O179:S179"/>
+    <mergeCell ref="O193:S193"/>
     <mergeCell ref="D102:E102"/>
     <mergeCell ref="C101:I101"/>
     <mergeCell ref="D121:E121"/>
     <mergeCell ref="C120:E120"/>
     <mergeCell ref="C144:O144"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C80:H80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="C84:I84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2116,15 +2221,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
@@ -2132,12 +2237,12 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2154,19 +2259,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -2191,24 +2294,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="8"/>
+      <c r="A4" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
@@ -2219,26 +2322,26 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28">
@@ -2249,22 +2352,22 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B33" t="s">

</xml_diff>